<commit_message>
desenvolvimento do circuito de alimentacao e emergencia
</commit_message>
<xml_diff>
--- a/descritivo/legendas.xlsx
+++ b/descritivo/legendas.xlsx
@@ -1,35 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Desktop\proj_MPM\MPM300\descritivo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\IPT\MPM300\desenhos\descritivo\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A9992B2-26D6-4AB5-BE72-0FFA61EA9035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7395" activeTab="4"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="regua de bornes" sheetId="1" r:id="rId1"/>
     <sheet name="contatores e relés" sheetId="6" r:id="rId2"/>
-    <sheet name="sensores analógicos" sheetId="3" r:id="rId3"/>
-    <sheet name="valvulas" sheetId="2" r:id="rId4"/>
+    <sheet name="valvulas" sheetId="2" r:id="rId3"/>
+    <sheet name="sensores analógicos" sheetId="3" r:id="rId4"/>
     <sheet name="referencias" sheetId="4" r:id="rId5"/>
     <sheet name="queda de tensão cabos" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="216">
   <si>
     <t>XB</t>
   </si>
@@ -127,48 +139,6 @@
     <t>transmissor (termo)</t>
   </si>
   <si>
-    <t>Nome (identificado)</t>
-  </si>
-  <si>
-    <t>K3</t>
-  </si>
-  <si>
-    <t>K4</t>
-  </si>
-  <si>
-    <t>K5</t>
-  </si>
-  <si>
-    <t>K6</t>
-  </si>
-  <si>
-    <t>K7</t>
-  </si>
-  <si>
-    <t>K8</t>
-  </si>
-  <si>
-    <t>Texto de função</t>
-  </si>
-  <si>
-    <t>contator bomba pesos</t>
-  </si>
-  <si>
-    <t>contator bomba varão</t>
-  </si>
-  <si>
-    <t>relé válvula pistão varão</t>
-  </si>
-  <si>
-    <t>relé válvula estabilizar varão</t>
-  </si>
-  <si>
-    <t>relé válvula pressão pesos</t>
-  </si>
-  <si>
-    <t>relé acionamento emergência (programa)</t>
-  </si>
-  <si>
     <t>KC1</t>
   </si>
   <si>
@@ -644,12 +614,87 @@
   </si>
   <si>
     <t>d18</t>
+  </si>
+  <si>
+    <t>XL</t>
+  </si>
+  <si>
+    <t>XRST</t>
+  </si>
+  <si>
+    <t>XLU</t>
+  </si>
+  <si>
+    <t>ENTRADA DA REDE</t>
+  </si>
+  <si>
+    <t>DISTRIBUICAO NO SECCIONAMENTO</t>
+  </si>
+  <si>
+    <t>DISTRIBUICAO PARA REGUA DE UTILIDADES E MOTOR DE POSICIONAMENTO</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>Y2</t>
+  </si>
+  <si>
+    <t>Y3</t>
+  </si>
+  <si>
+    <t>Y4</t>
+  </si>
+  <si>
+    <t>Y5</t>
+  </si>
+  <si>
+    <t>Y6</t>
+  </si>
+  <si>
+    <t>Y7</t>
+  </si>
+  <si>
+    <t>Y8</t>
+  </si>
+  <si>
+    <t>Y9</t>
+  </si>
+  <si>
+    <t>Y10</t>
+  </si>
+  <si>
+    <t>Y11</t>
+  </si>
+  <si>
+    <t>Y12</t>
+  </si>
+  <si>
+    <t>Y13</t>
+  </si>
+  <si>
+    <t>Y14</t>
+  </si>
+  <si>
+    <t>Y15</t>
+  </si>
+  <si>
+    <t>Y16</t>
+  </si>
+  <si>
+    <t>Y17</t>
+  </si>
+  <si>
+    <t>Y18</t>
+  </si>
+  <si>
+    <t>Y19</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -989,11 +1034,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E4:F18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="E4:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1019,7 +1064,7 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="5:6" x14ac:dyDescent="0.25">
@@ -1051,7 +1096,7 @@
         <v>6</v>
       </c>
       <c r="F10" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="5:6" x14ac:dyDescent="0.25">
@@ -1116,6 +1161,30 @@
       </c>
       <c r="F18" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>191</v>
+      </c>
+      <c r="F19" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="20" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>192</v>
+      </c>
+      <c r="F20" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="21" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>193</v>
+      </c>
+      <c r="F21" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -1124,11 +1193,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C3:L38"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5:H36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M5" sqref="M5:M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1146,449 +1215,449 @@
   <sheetData>
     <row r="3" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="G3" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="K3" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="G4" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="H4" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="K4" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="L4" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="G5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="H5" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="K5" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="L5" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="G6" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="H6" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="K6" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="L6" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="G7" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="H7" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="K7" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="L7" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="G8" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="H8" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="K8" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="L8" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="G9" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="H9" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="K9" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="L9" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="3:12" x14ac:dyDescent="0.25">
       <c r="G10" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="H10" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="K10" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="L10" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="3:12" x14ac:dyDescent="0.25">
       <c r="G11" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="H11" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="K11" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="L11" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="3:12" x14ac:dyDescent="0.25">
       <c r="G12" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="H12" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="K12" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="L12" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="3:12" x14ac:dyDescent="0.25">
       <c r="G13" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="H13" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="K13" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="L13" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="3:12" x14ac:dyDescent="0.25">
       <c r="G14" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="H14" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="K14" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="L14" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="3:12" x14ac:dyDescent="0.25">
       <c r="G15" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="H15" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="K15" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="L15" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16" spans="3:12" x14ac:dyDescent="0.25">
       <c r="G16" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="H16" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="K16" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="L16" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G17" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="H17" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="K17" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="L17" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G18" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="H18" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="K18" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="L18" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G19" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="H19" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="K19" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="L19" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G20" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="H20" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="K20" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="L20" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G21" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="H21" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="K21" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="L21" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G22" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="H22" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="K22" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="L22" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G23" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="H23" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="K23" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="L23" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G24" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="H24" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G25" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="H25" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G26" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="H26" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G27" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="H27" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G28" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="H28" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G29" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="H29" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G30" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="H30" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G31" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="H31" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G32" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="H32" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G33" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="H33" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G34" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="H34" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G35" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="H35" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
     </row>
     <row r="36" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G36" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="H36" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G37" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="H37" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
     </row>
     <row r="38" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G38" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="H38" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1597,7 +1666,200 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="G3:H22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4:F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="21.28515625" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G4" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="H4" t="str">
+        <f>CONCATENATE("solenóide ",'contatores e relés'!L5)</f>
+        <v>solenóide válvula 100A</v>
+      </c>
+    </row>
+    <row r="5" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G5" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="H5" t="str">
+        <f>CONCATENATE("solenóide ",'contatores e relés'!L6)</f>
+        <v>solenóide válvula 200A</v>
+      </c>
+    </row>
+    <row r="6" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G6" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="H6" t="str">
+        <f>CONCATENATE("solenóide ",'contatores e relés'!L7)</f>
+        <v>solenóide válvula 200B</v>
+      </c>
+    </row>
+    <row r="7" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G7" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="H7" t="str">
+        <f>CONCATENATE("solenóide ",'contatores e relés'!L8)</f>
+        <v>solenóide válvula 200C</v>
+      </c>
+    </row>
+    <row r="8" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G8" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="H8" t="str">
+        <f>CONCATENATE("solenóide ",'contatores e relés'!L9)</f>
+        <v>solenóide válvula 500A</v>
+      </c>
+    </row>
+    <row r="9" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G9" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="H9" t="str">
+        <f>CONCATENATE("solenóide ",'contatores e relés'!L10)</f>
+        <v>solenóide válvula 500B</v>
+      </c>
+    </row>
+    <row r="10" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G10" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="H10" t="str">
+        <f>CONCATENATE("solenóide ",'contatores e relés'!L11)</f>
+        <v>solenóide válvula 1000A</v>
+      </c>
+    </row>
+    <row r="11" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G11" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="H11" t="str">
+        <f>CONCATENATE("solenóide ",'contatores e relés'!L12)</f>
+        <v>solenóide válvula 1000B</v>
+      </c>
+    </row>
+    <row r="12" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G12" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="H12" t="str">
+        <f>CONCATENATE("solenóide ",'contatores e relés'!L13)</f>
+        <v>solenóide válvula 2000A</v>
+      </c>
+    </row>
+    <row r="13" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G13" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="H13" t="str">
+        <f>CONCATENATE("solenóide ",'contatores e relés'!L14)</f>
+        <v>solenóide válvula 2000B</v>
+      </c>
+    </row>
+    <row r="14" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G14" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="H14" t="str">
+        <f>CONCATENATE("solenóide ",'contatores e relés'!L15)</f>
+        <v>solenóide válvula 2000C</v>
+      </c>
+    </row>
+    <row r="15" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G15" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="H15" t="str">
+        <f>CONCATENATE("solenóide ",'contatores e relés'!L16)</f>
+        <v>solenóide válvula 2000D</v>
+      </c>
+    </row>
+    <row r="16" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G16" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="H16" t="str">
+        <f>CONCATENATE("solenóide ",'contatores e relés'!L17)</f>
+        <v>solenóide válvula 5000A</v>
+      </c>
+    </row>
+    <row r="17" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G17" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="H17" t="str">
+        <f>CONCATENATE("solenóide ",'contatores e relés'!L18)</f>
+        <v>solenóide válvula 5000B</v>
+      </c>
+    </row>
+    <row r="18" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G18" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="H18" t="str">
+        <f>CONCATENATE("solenóide ",'contatores e relés'!L19)</f>
+        <v>solenóide válvula 5000C</v>
+      </c>
+    </row>
+    <row r="19" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G19" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="H19" t="str">
+        <f>CONCATENATE("solenóide ",'contatores e relés'!L20)</f>
+        <v>solenóide válvula 5000D</v>
+      </c>
+    </row>
+    <row r="20" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G20" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="H20" t="str">
+        <f>CONCATENATE("solenóide ",'contatores e relés'!L21)</f>
+        <v>solenóide válvula cilindro varão</v>
+      </c>
+    </row>
+    <row r="21" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G21" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="H21" t="str">
+        <f>CONCATENATE("solenóide ",'contatores e relés'!L22)</f>
+        <v>solenóide válvula estabilizar varão</v>
+      </c>
+    </row>
+    <row r="22" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G22" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="H22" t="str">
+        <f>CONCATENATE("solenóide ",'contatores e relés'!L23)</f>
+        <v>solenóide válvula pressão dos pesos</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="F3:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1631,83 +1893,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E5:F11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="5" max="5" width="21.28515625" customWidth="1"/>
-    <col min="6" max="6" width="26.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="5" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="5:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="E6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="5:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="E11" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="D2:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1718,226 +1905,226 @@
   <sheetData>
     <row r="2" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="E2" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="I2" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="J2" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="E3" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="I3" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="J3" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="E4" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="I4" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="J4" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="E5" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="I5" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="J5" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="E6" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="I6" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="J6" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="E7" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="I7" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="J7" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E8" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="I8" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="J8" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="E9" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="I9" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="J9" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="E11" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="I11" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="J11" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="E12" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="I12" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="J12" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="E13" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="I13" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="J13" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="E14" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="I14" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="J14" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="E15" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="I15" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="J15" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="E16" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="I16" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="J16" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="E17" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="I17" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="J17" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="E18" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="I18" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="J18" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1946,7 +2133,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>